<commit_message>
Update Story test file
</commit_message>
<xml_diff>
--- a/Documents/Project Manage/Team Backlog.xlsx
+++ b/Documents/Project Manage/Team Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GithubProjects\Hippocampus\Documents\Project Manage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1A9A1B-30F7-4D0D-A253-6459348ACC09}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EBB0F8-FE44-44B4-8DDC-0AA60102E117}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="2865" windowWidth="15825" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Table 1</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>人设和LOGO，主角，女主角，典狱长的人设，</t>
+  </si>
+  <si>
+    <t>完成剧本</t>
   </si>
 </sst>
 </file>
@@ -1439,7 +1442,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -1549,37 +1552,53 @@
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+    <row r="7" spans="1:7" ht="23.25" customHeight="1">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.18</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="F7" s="3"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
+    <row r="8" spans="1:7" ht="80.099999999999994" customHeight="1">
+      <c r="A8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+    <row r="9" spans="1:7" ht="80.099999999999994" customHeight="1">
+      <c r="A9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="10"/>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="11"/>
+    <row r="10" spans="1:7" ht="80.099999999999994" customHeight="1">
+      <c r="A10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>

</xml_diff>